<commit_message>
Professeurs: CNE to CIN
</commit_message>
<xml_diff>
--- a/resources/professeurs.xlsx
+++ b/resources/professeurs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF1BDA4-3139-4516-B849-460E85B49962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2112A0B-F578-457B-A8EC-7053778D4758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D282FDAF-2FDC-4854-80D2-C8EA3F1CCD5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Rahali</t>
   </si>
   <si>
-    <t>CNE</t>
-  </si>
-  <si>
     <t>LastName</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Matiere2</t>
+  </si>
+  <si>
+    <t>CIN</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DE032-F837-48F3-9999-072D67E79C55}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,28 +526,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
       <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -561,19 +561,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,16 +587,16 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -610,16 +610,16 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -633,19 +633,19 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -659,16 +659,16 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,22 +676,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>